<commit_message>
add more test case
</commit_message>
<xml_diff>
--- a/TutorialNinja Test Cases .xlsx
+++ b/TutorialNinja Test Cases .xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MD. MOKHTAR\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MD. MOKHTAR\Documents\githubSystem\manual-testing-tutorialsninja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90366CEC-71C4-4B45-A140-C5D52671C064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9C24B8-9F07-4D53-80C5-73A78A10F0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -70,43 +70,272 @@
     <t>TC_001</t>
   </si>
   <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>Verify Registering an Account by providing only the mandatory filelds</t>
+  </si>
+  <si>
+    <t>open the Application URL https://tutorialsninja.com/demo/ in any browser</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>TC_002</t>
+  </si>
+  <si>
     <t>(TC_001)
-Registration Accoun t</t>
-  </si>
-  <si>
-    <t>Test Scenario</t>
-  </si>
-  <si>
-    <t>Verify Registering an Account by providing only the mandatory filelds</t>
-  </si>
-  <si>
-    <t>open the Application URL https://tutorialsninja.com/demo/ in any browser</t>
+Registration Account</t>
+  </si>
+  <si>
+    <t>Verify Registering an Account by providing all the fields</t>
+  </si>
+  <si>
+    <t>1.User should be Taken Register Account page
+2.User should get logged in, taken to Account Success page details and proper details should be displayed on the page
+3.User should be navigate to Account page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.User should get logged in, taken to Account Success page details and proper details should be displayed on the page
+2.User should be navigate to Account page</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>Verify proper notification messages are displayed for the mandatory fields , when you don't  provide any fields in the Register Account page and submit</t>
   </si>
   <si>
     <t xml:space="preserve">1. Click on My Account DropMenu
 2. Click on Register option
-3.Enter the new Account details into mandatory fileds only(first name, last name, E-mail,Telephone,Password,Password confirm)
+3.Don't enter anything into the fields
+5. Click on Continue button(ER-1)
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. The below warning messages should be displayed for the respective fields:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>First Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: "First Name must be between 1 and 32 characters!"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Last Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: "Last Name must be between 1 and 32 characters!"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E-Mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: "E-Mail Address does not appear to be valid!"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Telephone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: "Telephone must be between 3 and 32 characters!"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Password:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Password must be between 4 and 20 characters!"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Privacy Policy warning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: "You must agree to the Privacy Policy!"</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_004</t>
+  </si>
+  <si>
+    <t>Verify Registering Account when "yes" option is selected  for Newsletter field</t>
+  </si>
+  <si>
+    <t>1. Click on My Account DropMenu
+2. Click on Register option(ER-1)
+3.Enter the new Account details into mandatory fileds only(first name, last name,E-mail,Telephone,Password,Password confirm,Newsletter,and Privacy policy  field )
+4. Click on ' yes ' radio options for Newsletter
+5. Click on Continue button(ER-1)
+6.Click on continue button in the Account success page (ER-2)
+7.Click on ' subscribe/unsubscribe to newsletter' link(ER-3)</t>
+  </si>
+  <si>
+    <t>1. Click on My Account DropMenu
+2. Click on Register option(ER-1)
+3.Enter the new Account details into mandatory fileds only(first name, last name,E-mail,Telephone,Password,Password confirm)
+4.Selects the Privacy Policy
+5. Click on Continue button(ER-1)
+6.Click on continue button in the Account success page (ER-2)</t>
+  </si>
+  <si>
+    <t>1. Click on My Account DropMenu
+2. Click on Register option(ER-1)
+3.Enter the new Account details into mandatory fileds only(first name, last name,E-mail,Telephone,Password,Password confirm,Newsletter)
 4.Selects the Privacy Policy
 5. Click on Continue button
-6.Click on continue button in the Account success page </t>
-  </si>
-  <si>
-    <t>Not Applicable</t>
-  </si>
-  <si>
-    <t>1.User should be Taken Register Account page
-2.User should get logged in Account should be created and taken to Account Success page details
-3.User should be navigate to Account page</t>
-  </si>
-  <si>
-    <t>Pass</t>
+6.Click on continue button in the Account success page (ER-2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.User should get logged in, taken to Account Success page details and proper details should be displayed on the page
+2.User should be navigate to Account page
+3.' YES ' option should be displyed as selected by default in the Newsletter page</t>
+  </si>
+  <si>
+    <t>Verify Registering Account when "NO" option is selected  for Newsletter field</t>
+  </si>
+  <si>
+    <t>1. Click on My Account DropMenu
+2. Click on Register option(ER-1)
+3.Enter the new Account details into mandatory fileds only(first name, last name,E-mail,Telephone,Password,Password confirm,Newsletter,and Privacy policy  field )
+4. Click on ' NO ' radio options for Newsletter
+5. Click on Continue button(ER-1)
+6.Click on continue button in the Account success page (ER-2)
+7.Click on ' subscribe/unsubscribe to newsletter' link(ER-3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.User should get logged in, taken to Account Success page details and proper details should be displayed on the page
+2.User should be navigate to Account page
+3.' NO ' option should be displyed as selected by default in the Newsletter page</t>
+  </si>
+  <si>
+    <t>TC_005</t>
+  </si>
+  <si>
+    <t>TC_006</t>
+  </si>
+  <si>
+    <t>Verify different ways to navigating to 'Register Account' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option(ER-1)
+3. Click on 'My Account' Drop Menu
+4. Click on ' Login' option
+5. Click on 'Continue' button inside 'new customer' box(ER-1)
+6.Repeat steps 3 and 4
+7. Click on 'Register' optionm from the Right Column options(ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'Register Account' Page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +354,20 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -267,7 +510,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -289,9 +532,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -301,10 +541,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -612,29 +863,29 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H10" s="13"/>
+      <c r="H10" s="12"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H11" s="13"/>
+      <c r="H11" s="12"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H12" s="13"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H13" s="14"/>
+      <c r="H13" s="13"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
@@ -650,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +911,7 @@
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="34" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -675,7 +926,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>11</v>
@@ -705,100 +956,170 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>14</v>
+      <c r="B2" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+    <row r="3" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+    <row r="4" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+    <row r="5" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+    <row r="6" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+    <row r="7" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -1016,6 +1337,7 @@
       <c r="L22" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>